<commit_message>
Replaced hyphen (-) with elective (EL)
</commit_message>
<xml_diff>
--- a/public/composite-result-template.xlsx
+++ b/public/composite-result-template.xlsx
@@ -1,30 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macuser/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>S/N</t>
   </si>
@@ -68,22 +55,49 @@
     <t>GP</t>
   </si>
   <si>
-    <t>GPA</t>
+    <t>G.P.A.</t>
   </si>
   <si>
     <t>Jane Doe</t>
   </si>
   <si>
+    <t>52C</t>
+  </si>
+  <si>
+    <t>47D</t>
+  </si>
+  <si>
+    <t>35F</t>
+  </si>
+  <si>
+    <t>72A</t>
+  </si>
+  <si>
+    <t>82A</t>
+  </si>
+  <si>
+    <t>62B</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
     <t>John Doe</t>
   </si>
   <si>
+    <t>NIL</t>
+  </si>
+  <si>
+    <t>45D</t>
+  </si>
+  <si>
+    <t>40E</t>
+  </si>
+  <si>
+    <t>67B</t>
+  </si>
+  <si>
     <t>Jack Dorsy</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>NIL</t>
   </si>
   <si>
     <t>AB</t>
@@ -92,28 +106,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="4">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="9.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
-      <sz val="12"/>
+      <sz val="9.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -122,7 +132,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -131,63 +141,76 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
+    <border/>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -377,29 +400,20 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="15" width="12.83203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,30 +460,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="2">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="E2" s="2">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="F2" s="2">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="G2" s="2">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="H2" s="2">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="I2" s="2">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="J2" s="2">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -477,36 +491,36 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="4">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="4">
-        <v>2009457687</v>
-      </c>
-      <c r="D3" s="4">
-        <v>52</v>
-      </c>
-      <c r="E3" s="4">
-        <v>47</v>
-      </c>
-      <c r="F3" s="4">
-        <v>35</v>
-      </c>
-      <c r="G3" s="4">
-        <v>72</v>
-      </c>
-      <c r="H3" s="4">
-        <v>82</v>
-      </c>
-      <c r="I3" s="4">
-        <v>62</v>
+        <v>2.009457687E9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -514,36 +528,36 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="4">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C4" s="4">
-        <v>2009564738</v>
-      </c>
-      <c r="D4" s="4">
-        <v>62</v>
+        <v>2.009564738E9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="4">
-        <v>45</v>
-      </c>
-      <c r="G4" s="4">
-        <v>40</v>
-      </c>
-      <c r="H4" s="4">
-        <v>62</v>
+        <v>24</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="4">
-        <v>67</v>
+        <v>24</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -551,36 +565,36 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="4">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4">
-        <v>2009584732</v>
-      </c>
-      <c r="D5" s="4">
-        <v>62</v>
-      </c>
-      <c r="E5" s="4">
-        <v>45</v>
-      </c>
-      <c r="F5" s="4">
-        <v>45</v>
-      </c>
-      <c r="G5" s="4">
-        <v>40</v>
-      </c>
-      <c r="H5" s="4">
-        <v>62</v>
+        <v>2.009584732E9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="4">
-        <v>67</v>
+        <v>29</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -590,15 +604,15 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>